<commit_message>
Added the HotelSearch test cases in  testNg file
</commit_message>
<xml_diff>
--- a/src/main/java/com/hybridframework_Selenium/testdata/Test Suite1.xlsx
+++ b/src/main/java/com/hybridframework_Selenium/testdata/Test Suite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19815" windowHeight="3165" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19815" windowHeight="2685" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="Test Data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:L9"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="104">
   <si>
     <t>TCID</t>
   </si>
@@ -28,9 +27,6 @@
     <t>Runmode</t>
   </si>
   <si>
-    <t>LoginTest</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -121,9 +117,6 @@
     <t>loginlinkbtn</t>
   </si>
   <si>
-    <t>SignupTest</t>
-  </si>
-  <si>
     <t>testing for makemytrip signup page all possible scenarios</t>
   </si>
   <si>
@@ -160,27 +153,12 @@
     <t>signupemailtxtboxerrmsg|signupmobiletxtboxerrmsg|signuppasswdtxtboxerrmsg|afterloginusername|signuperrmsg</t>
   </si>
   <si>
-    <t>NormalSignUpTest</t>
-  </si>
-  <si>
-    <t>NormalLoginTest</t>
-  </si>
-  <si>
     <t>testing for normal flow of login form</t>
   </si>
   <si>
-    <t>Jakay</t>
-  </si>
-  <si>
     <t>testing for normal flow of sign up form</t>
   </si>
   <si>
-    <t>FlightSearchlistTestCase</t>
-  </si>
-  <si>
-    <t>testting for flight search listing page and verify the total price</t>
-  </si>
-  <si>
     <t>homepage.from.box</t>
   </si>
   <si>
@@ -272,6 +250,84 @@
   </si>
   <si>
     <t>listingpage.nameslist|listingpage.flightprice|flightreviewpage.finalprice</t>
+  </si>
+  <si>
+    <t>verifyReviewPageGrandTotal</t>
+  </si>
+  <si>
+    <t>flightreviewpage.basefire|flightreviewpage.feesurcharges|flightreviewpage.grandtotal</t>
+  </si>
+  <si>
+    <t>directInput</t>
+  </si>
+  <si>
+    <t>jakay577@gmail.com</t>
+  </si>
+  <si>
+    <t>976556767</t>
+  </si>
+  <si>
+    <t>7889</t>
+  </si>
+  <si>
+    <t>signUpPageTestcases</t>
+  </si>
+  <si>
+    <t>loginTestwithDifferentscenarios</t>
+  </si>
+  <si>
+    <t>homepage.header.hotellink</t>
+  </si>
+  <si>
+    <t>Online Hotel Booking for Cheap, Budget &amp; Luxury Hotels in India | MakeMyTrip.com</t>
+  </si>
+  <si>
+    <t>homepage.hotel.city.hoteltxt</t>
+  </si>
+  <si>
+    <t>homepage.hotel.city.hoteloptions</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>homepage.hotel.roomguests</t>
+  </si>
+  <si>
+    <t>2|4|2</t>
+  </si>
+  <si>
+    <t>testing for flight search listing page and verify the total price</t>
+  </si>
+  <si>
+    <t>testing for hotel search listing page and verify the final price</t>
+  </si>
+  <si>
+    <t>9985652</t>
+  </si>
+  <si>
+    <t>hotelSearchlistTestCase</t>
+  </si>
+  <si>
+    <t>chooseChildrenswiththeirAge</t>
+  </si>
+  <si>
+    <t>normalFlowLoginTestcase</t>
+  </si>
+  <si>
+    <t>normalSignUpTestcase</t>
+  </si>
+  <si>
+    <t>flightSearchlistTestCase</t>
+  </si>
+  <si>
+    <t>25-October 2017</t>
+  </si>
+  <si>
+    <t>homepage.hotel.getchlOutselecteddate</t>
+  </si>
+  <si>
+    <t>27-November 2017</t>
   </si>
 </sst>
 </file>
@@ -294,7 +350,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -337,8 +393,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -361,26 +423,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -389,7 +431,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -398,13 +440,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -700,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -726,57 +772,68 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>93</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -786,10 +843,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -809,44 +866,44 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="6" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="6"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="6" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="6" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
@@ -859,100 +916,100 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="6" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="6"/>
+        <v>30</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>31</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="6" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="6" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="6" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>43</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D10" s="6"/>
       <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5">
-      <c r="A11" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
+      <c r="A11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
@@ -965,128 +1022,128 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>46</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
+      <c r="A21" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="7"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="7" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="s">
@@ -1099,7 +1156,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="7" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
@@ -1112,7 +1169,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="7" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
@@ -1125,87 +1182,87 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="7" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E25" s="7"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="7" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="7" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>11</v>
+      <c r="E27" s="12" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="7" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="E28" s="7"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="7" t="s">
-        <v>48</v>
+        <v>98</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>33</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D29" s="7"/>
       <c r="E29" s="7"/>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
+      <c r="A30" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
@@ -1218,416 +1275,616 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>6</v>
+        <v>80</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E34" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>11</v>
+      <c r="E35" s="14" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="2" t="s">
-        <v>47</v>
+        <v>99</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>46</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="D39" s="2"/>
       <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
+      <c r="A40" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B40" s="8"/>
+      <c r="C40" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="8"/>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="8"/>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B42" s="8"/>
+      <c r="C42" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E42" s="8"/>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E43" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E41" s="8"/>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B42" s="8"/>
-      <c r="C42" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E42" s="8"/>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="9" t="s">
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E44" s="8"/>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E43" s="8"/>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="9" t="s">
+      <c r="E46" s="8"/>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D47" s="8"/>
+      <c r="E47" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="D44" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="E45" s="8"/>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="D46" s="11" t="s">
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D48" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E46" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B47" s="8"/>
-      <c r="C47" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E47" s="8"/>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D48" s="11"/>
-      <c r="E48" s="12" t="s">
-        <v>63</v>
-      </c>
+      <c r="E48" s="8"/>
     </row>
     <row r="49" spans="1:5">
-      <c r="A49" s="10" t="s">
-        <v>52</v>
+      <c r="A49" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="E49" s="8"/>
+        <v>58</v>
+      </c>
+      <c r="D49" s="8"/>
+      <c r="E49" s="10" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="50" spans="1:5">
-      <c r="A50" s="10" t="s">
-        <v>52</v>
+      <c r="A50" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D50" s="8"/>
-      <c r="E50" s="13" t="s">
-        <v>74</v>
+      <c r="E50" s="10" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:5">
-      <c r="A51" s="10" t="s">
-        <v>52</v>
+      <c r="A51" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="8" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D51" s="8"/>
-      <c r="E51" s="13" t="s">
-        <v>75</v>
+      <c r="E51" s="10" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:5">
-      <c r="A52" s="10" t="s">
-        <v>52</v>
+      <c r="A52" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D52" s="8"/>
-      <c r="E52" s="13" t="s">
-        <v>75</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="E52" s="8"/>
     </row>
     <row r="53" spans="1:5">
-      <c r="A53" s="10" t="s">
-        <v>52</v>
+      <c r="A53" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8" t="s">
-        <v>6</v>
+        <v>62</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="E53" s="8"/>
     </row>
     <row r="54" spans="1:5">
-      <c r="A54" s="10" t="s">
-        <v>52</v>
+      <c r="A54" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="8" t="s">
-        <v>69</v>
+        <v>5</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E54" s="8"/>
     </row>
     <row r="55" spans="1:5">
-      <c r="A55" s="10" t="s">
-        <v>52</v>
+      <c r="A55" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E55" s="8"/>
+        <v>64</v>
+      </c>
+      <c r="D55" s="8"/>
+      <c r="E55" s="8" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="56" spans="1:5">
-      <c r="A56" s="10" t="s">
-        <v>52</v>
+      <c r="A56" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D56" s="8"/>
-      <c r="E56" s="8" t="s">
-        <v>72</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5">
-      <c r="A57" s="10" t="s">
-        <v>52</v>
+      <c r="A57" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="8" t="s">
-        <v>6</v>
+        <v>70</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E57" s="8"/>
     </row>
     <row r="58" spans="1:5">
-      <c r="A58" s="10" t="s">
-        <v>52</v>
+      <c r="A58" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E58" s="8"/>
     </row>
     <row r="59" spans="1:5">
-      <c r="A59" s="10" t="s">
-        <v>52</v>
+      <c r="A59" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="B59" s="8"/>
       <c r="C59" s="8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E59" s="8"/>
     </row>
     <row r="60" spans="1:5">
-      <c r="A60" s="10" t="s">
-        <v>52</v>
+      <c r="A60" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="8" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E60" s="8"/>
+        <v>77</v>
+      </c>
+      <c r="E60" s="11" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="61" spans="1:5">
-      <c r="A61" s="10" t="s">
-        <v>52</v>
+      <c r="A61" s="8" t="s">
+        <v>100</v>
       </c>
       <c r="B61" s="8"/>
       <c r="C61" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="E61" s="14" t="s">
-        <v>83</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E61" s="11"/>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D62" s="11"/>
+      <c r="E62" s="11"/>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B63" s="15"/>
+      <c r="C63" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E63" s="16"/>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B64" s="15"/>
+      <c r="C64" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E64" s="15"/>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B65" s="15"/>
+      <c r="C65" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="E65" s="15"/>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B66" s="15"/>
+      <c r="C66" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D66" s="15"/>
+      <c r="E66" s="15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B67" s="15"/>
+      <c r="C67" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E67" s="15"/>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B68" s="15"/>
+      <c r="C68" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E68" s="15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B69" s="15"/>
+      <c r="C69" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D69" s="15"/>
+      <c r="E69" s="17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B70" s="15"/>
+      <c r="C70" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E70" s="17"/>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B71" s="15"/>
+      <c r="C71" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="D71" s="15"/>
+      <c r="E71" s="17" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B72" s="15"/>
+      <c r="C72" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E72" s="18"/>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B73" s="15"/>
+      <c r="C73" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D73" s="15"/>
+      <c r="E73" s="18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B74" s="15"/>
+      <c r="C74" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="D74" s="15"/>
+      <c r="E74" s="18" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B75" s="15"/>
+      <c r="C75" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D75" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E75" s="18"/>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B76" s="15"/>
+      <c r="C76" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E76" s="18"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E26" r:id="rId1"/>
+    <hyperlink ref="E27" r:id="rId2"/>
+    <hyperlink ref="E34" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1635,16 +1892,16 @@
     <col min="1" max="1" width="20.42578125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="29.42578125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17.28515625" hidden="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="16" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
-        <v>3</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1652,79 +1909,79 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
-        <v>34</v>
+        <v>84</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -1738,123 +1995,40 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C16">
-        <v>9565235330</v>
-      </c>
-      <c r="D16">
-        <v>123456789</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>45</v>
+        <v>24</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="B20" r:id="rId5"/>
-    <hyperlink ref="C20" r:id="rId6"/>
+    <hyperlink ref="C5" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B4" r:id="rId3"/>
+    <hyperlink ref="B8" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId7"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added the batch file and pom file changes send the report automatically
</commit_message>
<xml_diff>
--- a/src/main/java/com/hybridframework_Selenium/testdata/Test Suite1.xlsx
+++ b/src/main/java/com/hybridframework_Selenium/testdata/Test Suite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19815" windowHeight="2685" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19815" windowHeight="2685" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Test Data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1:L7"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="108">
   <si>
     <t>TCID</t>
   </si>
@@ -328,6 +329,18 @@
   </si>
   <si>
     <t>27-November 2017</t>
+  </si>
+  <si>
+    <t>homepage.hotel.outsidefield</t>
+  </si>
+  <si>
+    <t>Please enter a valid Email Address</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>SKIP</t>
   </si>
 </sst>
 </file>
@@ -843,9 +856,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E76"/>
+  <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+    <sheetView topLeftCell="A57" workbookViewId="0">
       <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
@@ -1786,7 +1799,7 @@
         <v>5</v>
       </c>
       <c r="D70" s="15" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="E70" s="17"/>
     </row>
@@ -1796,12 +1809,12 @@
       </c>
       <c r="B71" s="15"/>
       <c r="C71" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D71" s="15"/>
-      <c r="E71" s="17" t="s">
-        <v>103</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="E71" s="17"/>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="15" t="s">
@@ -1809,12 +1822,12 @@
       </c>
       <c r="B72" s="15"/>
       <c r="C72" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D72" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E72" s="18"/>
+        <v>55</v>
+      </c>
+      <c r="D72" s="15"/>
+      <c r="E72" s="17" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="15" t="s">
@@ -1822,12 +1835,12 @@
       </c>
       <c r="B73" s="15"/>
       <c r="C73" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D73" s="15"/>
-      <c r="E73" s="18" t="s">
-        <v>67</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="E73" s="18"/>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="15" t="s">
@@ -1835,11 +1848,11 @@
       </c>
       <c r="B74" s="15"/>
       <c r="C74" s="15" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="D74" s="15"/>
       <c r="E74" s="18" t="s">
-        <v>92</v>
+        <v>67</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -1848,12 +1861,12 @@
       </c>
       <c r="B75" s="15"/>
       <c r="C75" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="D75" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E75" s="18"/>
+        <v>97</v>
+      </c>
+      <c r="D75" s="15"/>
+      <c r="E75" s="18" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="15" t="s">
@@ -1861,12 +1874,25 @@
       </c>
       <c r="B76" s="15"/>
       <c r="C76" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E76" s="18"/>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B77" s="15"/>
+      <c r="C77" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D76" s="15" t="s">
+      <c r="D77" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E76" s="18"/>
+      <c r="E77" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1883,8 +1909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1893,8 +1919,8 @@
     <col min="2" max="2" width="29.42578125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="17.28515625" hidden="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="16" customWidth="1" collapsed="1"/>
   </cols>
@@ -1927,6 +1953,9 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
+      <c r="E3" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
@@ -1938,6 +1967,9 @@
       <c r="C4" t="s">
         <v>25</v>
       </c>
+      <c r="E4" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
@@ -1949,6 +1981,9 @@
       <c r="C5" s="4" t="s">
         <v>43</v>
       </c>
+      <c r="E5" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
@@ -1958,6 +1993,9 @@
       <c r="C6" s="5" t="s">
         <v>26</v>
       </c>
+      <c r="E6" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
@@ -1967,6 +2005,9 @@
       <c r="C7" s="5" t="s">
         <v>26</v>
       </c>
+      <c r="E7" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
@@ -1977,6 +2018,9 @@
       </c>
       <c r="C8" s="5" t="s">
         <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2019,6 +2063,12 @@
       </c>
       <c r="C12" s="5" t="s">
         <v>95</v>
+      </c>
+      <c r="E12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F12" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes for test cases and added the batch file.
</commit_message>
<xml_diff>
--- a/src/main/java/com/hybridframework_Selenium/testdata/Test Suite1.xlsx
+++ b/src/main/java/com/hybridframework_Selenium/testdata/Test Suite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19815" windowHeight="2685" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19815" windowHeight="2685" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,11 @@
     <sheet name="Test Data" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <oleSize ref="A1:L7"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="114">
   <si>
     <t>TCID</t>
   </si>
@@ -325,22 +324,40 @@
     <t>25-October 2017</t>
   </si>
   <si>
-    <t>homepage.hotel.getchlOutselecteddate</t>
-  </si>
-  <si>
-    <t>27-November 2017</t>
-  </si>
-  <si>
-    <t>homepage.hotel.outsidefield</t>
-  </si>
-  <si>
-    <t>Please enter a valid Email Address</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>SKIP</t>
+    <t>chooseDateReturn</t>
+  </si>
+  <si>
+    <t>waitForTextPresent</t>
+  </si>
+  <si>
+    <t>scrollDownUntilCountMatch</t>
+  </si>
+  <si>
+    <t>listingpage.hotelnamelist</t>
+  </si>
+  <si>
+    <t>28-October 2017</t>
+  </si>
+  <si>
+    <t>listingpage.hotelpageheading</t>
+  </si>
+  <si>
+    <t>Hotels in Bangalore</t>
+  </si>
+  <si>
+    <t>Ramada Encore</t>
+  </si>
+  <si>
+    <t>listingpage.hotelnamelist|listingpage.hotelpricelist|listingpage.hotel.list.allImages</t>
+  </si>
+  <si>
+    <t>selectGivenHotelInalist</t>
+  </si>
+  <si>
+    <t>verifyTextPresent</t>
+  </si>
+  <si>
+    <t>hotel.viewpage.hotelname</t>
   </si>
 </sst>
 </file>
@@ -762,7 +779,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -856,22 +873,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:F80"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="E73" sqref="E73"/>
+    <sheetView tabSelected="1" topLeftCell="C59" workbookViewId="0">
+      <selection activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="42.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="76.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -887,8 +905,11 @@
       <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="6" t="s">
         <v>85</v>
       </c>
@@ -900,8 +921,9 @@
         <v>19</v>
       </c>
       <c r="E2" s="6"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="6" t="s">
         <v>85</v>
       </c>
@@ -913,8 +935,9 @@
         <v>20</v>
       </c>
       <c r="E3" s="6"/>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="6" t="s">
         <v>85</v>
       </c>
@@ -926,8 +949,9 @@
         <v>22</v>
       </c>
       <c r="E4" s="6"/>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="6" t="s">
         <v>85</v>
       </c>
@@ -939,8 +963,9 @@
         <v>22</v>
       </c>
       <c r="E5" s="6"/>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" s="6"/>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="6" t="s">
         <v>85</v>
       </c>
@@ -954,8 +979,9 @@
       <c r="E6" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="6" t="s">
         <v>85</v>
       </c>
@@ -969,8 +995,9 @@
       <c r="E7" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="6" t="s">
         <v>85</v>
       </c>
@@ -982,8 +1009,9 @@
         <v>32</v>
       </c>
       <c r="E8" s="6"/>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="6" t="s">
         <v>85</v>
       </c>
@@ -995,8 +1023,9 @@
         <v>41</v>
       </c>
       <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="6" t="s">
         <v>85</v>
       </c>
@@ -1006,8 +1035,9 @@
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
         <v>84</v>
       </c>
@@ -1019,8 +1049,9 @@
         <v>19</v>
       </c>
       <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" s="2"/>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
         <v>84</v>
       </c>
@@ -1032,8 +1063,9 @@
         <v>20</v>
       </c>
       <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
         <v>84</v>
       </c>
@@ -1045,8 +1077,9 @@
         <v>34</v>
       </c>
       <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
         <v>84</v>
       </c>
@@ -1058,8 +1091,9 @@
         <v>34</v>
       </c>
       <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
         <v>84</v>
       </c>
@@ -1073,8 +1107,9 @@
       <c r="E15" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
         <v>84</v>
       </c>
@@ -1088,8 +1123,9 @@
       <c r="E16" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
         <v>84</v>
       </c>
@@ -1103,8 +1139,9 @@
       <c r="E17" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
         <v>84</v>
       </c>
@@ -1116,8 +1153,9 @@
         <v>38</v>
       </c>
       <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
         <v>84</v>
       </c>
@@ -1129,8 +1167,9 @@
         <v>44</v>
       </c>
       <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
         <v>84</v>
       </c>
@@ -1140,8 +1179,9 @@
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="7" t="s">
         <v>98</v>
       </c>
@@ -1153,8 +1193,9 @@
         <v>19</v>
       </c>
       <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="7" t="s">
         <v>98</v>
       </c>
@@ -1166,8 +1207,9 @@
         <v>20</v>
       </c>
       <c r="E22" s="7"/>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" s="7" t="s">
         <v>98</v>
       </c>
@@ -1179,8 +1221,9 @@
         <v>21</v>
       </c>
       <c r="E23" s="7"/>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" s="7"/>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" s="7" t="s">
         <v>98</v>
       </c>
@@ -1192,8 +1235,9 @@
         <v>22</v>
       </c>
       <c r="E24" s="7"/>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="7" t="s">
         <v>98</v>
       </c>
@@ -1205,8 +1249,9 @@
         <v>22</v>
       </c>
       <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" s="7" t="s">
         <v>98</v>
       </c>
@@ -1220,8 +1265,9 @@
       <c r="E26" s="12" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="7" t="s">
         <v>98</v>
       </c>
@@ -1235,8 +1281,9 @@
       <c r="E27" s="12" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" s="7" t="s">
         <v>98</v>
       </c>
@@ -1248,8 +1295,9 @@
         <v>32</v>
       </c>
       <c r="E28" s="7"/>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" s="7" t="s">
         <v>98</v>
       </c>
@@ -1259,8 +1307,9 @@
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" s="2" t="s">
         <v>99</v>
       </c>
@@ -1272,8 +1321,9 @@
         <v>19</v>
       </c>
       <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="2" t="s">
         <v>99</v>
       </c>
@@ -1285,8 +1335,9 @@
         <v>20</v>
       </c>
       <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" s="2" t="s">
         <v>99</v>
       </c>
@@ -1298,8 +1349,9 @@
         <v>34</v>
       </c>
       <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" s="2" t="s">
         <v>99</v>
       </c>
@@ -1311,8 +1363,9 @@
         <v>34</v>
       </c>
       <c r="E33" s="2"/>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="2" t="s">
         <v>99</v>
       </c>
@@ -1326,8 +1379,9 @@
       <c r="E34" s="13" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" s="2" t="s">
         <v>99</v>
       </c>
@@ -1341,8 +1395,9 @@
       <c r="E35" s="14" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" s="2" t="s">
         <v>99</v>
       </c>
@@ -1356,8 +1411,9 @@
       <c r="E36" s="14" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="2" t="s">
         <v>99</v>
       </c>
@@ -1369,8 +1425,9 @@
         <v>38</v>
       </c>
       <c r="E37" s="2"/>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" s="2" t="s">
         <v>99</v>
       </c>
@@ -1382,8 +1439,9 @@
         <v>44</v>
       </c>
       <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" s="2" t="s">
         <v>99</v>
       </c>
@@ -1393,8 +1451,9 @@
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="8" t="s">
         <v>100</v>
       </c>
@@ -1406,8 +1465,9 @@
         <v>19</v>
       </c>
       <c r="E40" s="8"/>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="F40" s="8"/>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41" s="8" t="s">
         <v>100</v>
       </c>
@@ -1419,8 +1479,9 @@
         <v>20</v>
       </c>
       <c r="E41" s="8"/>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="F41" s="8"/>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="8" t="s">
         <v>100</v>
       </c>
@@ -1432,8 +1493,9 @@
         <v>47</v>
       </c>
       <c r="E42" s="8"/>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="F42" s="8"/>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43" s="8" t="s">
         <v>100</v>
       </c>
@@ -1447,8 +1509,9 @@
       <c r="E43" s="8" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="F43" s="8"/>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44" s="8" t="s">
         <v>100</v>
       </c>
@@ -1460,8 +1523,9 @@
         <v>51</v>
       </c>
       <c r="E44" s="8"/>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="F44" s="8"/>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45" s="8" t="s">
         <v>100</v>
       </c>
@@ -1475,8 +1539,9 @@
       <c r="E45" s="8" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="8" t="s">
         <v>100</v>
       </c>
@@ -1488,8 +1553,9 @@
         <v>54</v>
       </c>
       <c r="E46" s="8"/>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="F46" s="8"/>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47" s="8" t="s">
         <v>100</v>
       </c>
@@ -1501,8 +1567,9 @@
       <c r="E47" s="9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="F47" s="8"/>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48" s="8" t="s">
         <v>100</v>
       </c>
@@ -1514,8 +1581,9 @@
         <v>57</v>
       </c>
       <c r="E48" s="8"/>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="F48" s="8"/>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49" s="8" t="s">
         <v>100</v>
       </c>
@@ -1527,8 +1595,9 @@
       <c r="E49" s="10" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="F49" s="8"/>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="8" t="s">
         <v>100</v>
       </c>
@@ -1540,8 +1609,9 @@
       <c r="E50" s="10" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="F50" s="8"/>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51" s="8" t="s">
         <v>100</v>
       </c>
@@ -1553,8 +1623,9 @@
       <c r="E51" s="10" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="F51" s="8"/>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52" s="8" t="s">
         <v>100</v>
       </c>
@@ -1566,8 +1637,9 @@
         <v>61</v>
       </c>
       <c r="E52" s="8"/>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="F52" s="8"/>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="8" t="s">
         <v>100</v>
       </c>
@@ -1579,8 +1651,9 @@
         <v>57</v>
       </c>
       <c r="E53" s="8"/>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" spans="1:6">
       <c r="A54" s="8" t="s">
         <v>100</v>
       </c>
@@ -1592,8 +1665,9 @@
         <v>63</v>
       </c>
       <c r="E54" s="8"/>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="F54" s="8"/>
+    </row>
+    <row r="55" spans="1:6">
       <c r="A55" s="8" t="s">
         <v>100</v>
       </c>
@@ -1605,8 +1679,9 @@
       <c r="E55" s="8" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="F55" s="8"/>
+    </row>
+    <row r="56" spans="1:6">
       <c r="A56" s="8" t="s">
         <v>100</v>
       </c>
@@ -1618,8 +1693,9 @@
         <v>66</v>
       </c>
       <c r="E56" s="8"/>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="F56" s="8"/>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" s="8" t="s">
         <v>100</v>
       </c>
@@ -1631,8 +1707,9 @@
         <v>69</v>
       </c>
       <c r="E57" s="8"/>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="F57" s="8"/>
+    </row>
+    <row r="58" spans="1:6">
       <c r="A58" s="8" t="s">
         <v>100</v>
       </c>
@@ -1644,8 +1721,9 @@
         <v>72</v>
       </c>
       <c r="E58" s="8"/>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="F58" s="8"/>
+    </row>
+    <row r="59" spans="1:6">
       <c r="A59" s="8" t="s">
         <v>100</v>
       </c>
@@ -1657,8 +1735,9 @@
         <v>71</v>
       </c>
       <c r="E59" s="8"/>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="F59" s="8"/>
+    </row>
+    <row r="60" spans="1:6">
       <c r="A60" s="8" t="s">
         <v>100</v>
       </c>
@@ -1672,8 +1751,9 @@
       <c r="E60" s="11" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="F60" s="8"/>
+    </row>
+    <row r="61" spans="1:6">
       <c r="A61" s="8" t="s">
         <v>100</v>
       </c>
@@ -1685,8 +1765,9 @@
         <v>79</v>
       </c>
       <c r="E61" s="11"/>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="F61" s="8"/>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" s="8" t="s">
         <v>100</v>
       </c>
@@ -1696,8 +1777,9 @@
       </c>
       <c r="D62" s="11"/>
       <c r="E62" s="11"/>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="F62" s="8"/>
+    </row>
+    <row r="63" spans="1:6">
       <c r="A63" s="15" t="s">
         <v>96</v>
       </c>
@@ -1709,8 +1791,9 @@
         <v>19</v>
       </c>
       <c r="E63" s="16"/>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="F63" s="16"/>
+    </row>
+    <row r="64" spans="1:6">
       <c r="A64" s="15" t="s">
         <v>96</v>
       </c>
@@ -1722,8 +1805,9 @@
         <v>20</v>
       </c>
       <c r="E64" s="15"/>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="F64" s="16"/>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" s="15" t="s">
         <v>96</v>
       </c>
@@ -1735,8 +1819,9 @@
         <v>86</v>
       </c>
       <c r="E65" s="15"/>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="F65" s="16"/>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" s="15" t="s">
         <v>96</v>
       </c>
@@ -1748,8 +1833,9 @@
       <c r="E66" s="15" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="F66" s="16"/>
+    </row>
+    <row r="67" spans="1:6">
       <c r="A67" s="15" t="s">
         <v>96</v>
       </c>
@@ -1761,8 +1847,9 @@
         <v>88</v>
       </c>
       <c r="E67" s="15"/>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="F67" s="16"/>
+    </row>
+    <row r="68" spans="1:6">
       <c r="A68" s="15" t="s">
         <v>96</v>
       </c>
@@ -1776,8 +1863,9 @@
       <c r="E68" s="15" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="F68" s="16"/>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" s="15" t="s">
         <v>96</v>
       </c>
@@ -1789,21 +1877,23 @@
       <c r="E69" s="17" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="F69" s="16"/>
+    </row>
+    <row r="70" spans="1:6">
       <c r="A70" s="15" t="s">
         <v>96</v>
       </c>
       <c r="B70" s="15"/>
       <c r="C70" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D70" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E70" s="17"/>
-    </row>
-    <row r="71" spans="1:5">
+        <v>102</v>
+      </c>
+      <c r="D70" s="15"/>
+      <c r="E70" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="F70" s="16"/>
+    </row>
+    <row r="71" spans="1:6">
       <c r="A71" s="15" t="s">
         <v>96</v>
       </c>
@@ -1812,87 +1902,144 @@
         <v>5</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="E71" s="17"/>
-    </row>
-    <row r="72" spans="1:5">
+        <v>91</v>
+      </c>
+      <c r="E71" s="18"/>
+      <c r="F71" s="16"/>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" s="15" t="s">
         <v>96</v>
       </c>
       <c r="B72" s="15"/>
       <c r="C72" s="15" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D72" s="15"/>
-      <c r="E72" s="17" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="E72" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="F72" s="16"/>
+    </row>
+    <row r="73" spans="1:6">
       <c r="A73" s="15" t="s">
         <v>96</v>
       </c>
       <c r="B73" s="15"/>
       <c r="C73" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D73" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E73" s="18"/>
-    </row>
-    <row r="74" spans="1:5">
+        <v>97</v>
+      </c>
+      <c r="D73" s="15"/>
+      <c r="E73" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="F73" s="16"/>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74" s="15" t="s">
         <v>96</v>
       </c>
       <c r="B74" s="15"/>
       <c r="C74" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D74" s="15"/>
-      <c r="E74" s="18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
+        <v>62</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="E74" s="18"/>
+      <c r="F74" s="16"/>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75" s="15" t="s">
         <v>96</v>
       </c>
       <c r="B75" s="15"/>
       <c r="C75" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="D75" s="15"/>
-      <c r="E75" s="18" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
+        <v>5</v>
+      </c>
+      <c r="D75" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="E75" s="18"/>
+      <c r="F75" s="16"/>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76" s="15" t="s">
         <v>96</v>
       </c>
       <c r="B76" s="15"/>
       <c r="C76" s="15" t="s">
-        <v>62</v>
+        <v>103</v>
       </c>
       <c r="D76" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E76" s="18"/>
-    </row>
-    <row r="77" spans="1:5">
+        <v>107</v>
+      </c>
+      <c r="E76" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="F76" s="16"/>
+    </row>
+    <row r="77" spans="1:6">
       <c r="A77" s="15" t="s">
         <v>96</v>
       </c>
       <c r="B77" s="15"/>
       <c r="C77" s="15" t="s">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="D77" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="E77" s="18"/>
+        <v>105</v>
+      </c>
+      <c r="E77" s="17"/>
+      <c r="F77" s="16"/>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B78" s="15"/>
+      <c r="C78" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="E78" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F78" s="16"/>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B79" s="15"/>
+      <c r="C79" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D79" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="E79" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F79" s="16"/>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B80" s="15"/>
+      <c r="C80" s="15" t="s">
+        <v>112</v>
+      </c>
+      <c r="D80" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="E80" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F80" s="16"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1909,8 +2056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1919,7 +2066,7 @@
     <col min="2" max="2" width="29.42578125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="31.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="17.28515625" hidden="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="16" customWidth="1" collapsed="1"/>
@@ -1953,9 +2100,6 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
-      <c r="E3" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
@@ -1967,9 +2111,6 @@
       <c r="C4" t="s">
         <v>25</v>
       </c>
-      <c r="E4" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
@@ -1981,9 +2122,6 @@
       <c r="C5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E5" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
@@ -1993,9 +2131,6 @@
       <c r="C6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E6" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
@@ -2005,9 +2140,6 @@
       <c r="C7" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E7" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
@@ -2018,9 +2150,6 @@
       </c>
       <c r="C8" s="5" t="s">
         <v>27</v>
-      </c>
-      <c r="E8" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2063,12 +2192,6 @@
       </c>
       <c r="C12" s="5" t="s">
         <v>95</v>
-      </c>
-      <c r="E12" t="s">
-        <v>105</v>
-      </c>
-      <c r="F12" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test cases is modified and completed the hotel booking test case.
</commit_message>
<xml_diff>
--- a/src/main/java/com/hybridframework_Selenium/testdata/Test Suite1.xlsx
+++ b/src/main/java/com/hybridframework_Selenium/testdata/Test Suite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19815" windowHeight="2685" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19815" windowHeight="2685" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="151">
   <si>
     <t>TCID</t>
   </si>
@@ -90,9 +90,6 @@
     <t>close</t>
   </si>
   <si>
-    <t>jakay</t>
-  </si>
-  <si>
     <t>hjkhjhdjd^7</t>
   </si>
   <si>
@@ -303,9 +300,6 @@
     <t>testing for hotel search listing page and verify the final price</t>
   </si>
   <si>
-    <t>9985652</t>
-  </si>
-  <si>
     <t>hotelSearchlistTestCase</t>
   </si>
   <si>
@@ -321,43 +315,160 @@
     <t>flightSearchlistTestCase</t>
   </si>
   <si>
-    <t>25-October 2017</t>
-  </si>
-  <si>
     <t>chooseDateReturn</t>
   </si>
   <si>
     <t>waitForTextPresent</t>
   </si>
   <si>
-    <t>scrollDownUntilCountMatch</t>
-  </si>
-  <si>
-    <t>listingpage.hotelnamelist</t>
-  </si>
-  <si>
-    <t>28-October 2017</t>
-  </si>
-  <si>
     <t>listingpage.hotelpageheading</t>
   </si>
   <si>
     <t>Hotels in Bangalore</t>
   </si>
   <si>
-    <t>Ramada Encore</t>
-  </si>
-  <si>
-    <t>listingpage.hotelnamelist|listingpage.hotelpricelist|listingpage.hotel.list.allImages</t>
-  </si>
-  <si>
-    <t>selectGivenHotelInalist</t>
-  </si>
-  <si>
     <t>verifyTextPresent</t>
   </si>
   <si>
     <t>hotel.viewpage.hotelname</t>
+  </si>
+  <si>
+    <t>clickOngivenName</t>
+  </si>
+  <si>
+    <t>switchtoWindow</t>
+  </si>
+  <si>
+    <t>hotel.viewpage.roomonly.bookbtn</t>
+  </si>
+  <si>
+    <t>verify_BookingConfirmationDetailsprice</t>
+  </si>
+  <si>
+    <t>selectDropdown</t>
+  </si>
+  <si>
+    <t>booking.confirmationpage.titledropdown</t>
+  </si>
+  <si>
+    <t>booking.confirmationpage.firstnametxtbox</t>
+  </si>
+  <si>
+    <t>booking.confirmationpage.lastnametxtbox</t>
+  </si>
+  <si>
+    <t>booking.confirmationpage.emailtxtbox</t>
+  </si>
+  <si>
+    <t>booking.confirmationpage.contactnotxtbox</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>Ms.</t>
+  </si>
+  <si>
+    <t>moveCusoronElement</t>
+  </si>
+  <si>
+    <t>waitForElementPresent</t>
+  </si>
+  <si>
+    <t>waitForInvisibility</t>
+  </si>
+  <si>
+    <t>homepage.datepicker.leftside.monthyear</t>
+  </si>
+  <si>
+    <t>homepage.hotel.roomguests.done</t>
+  </si>
+  <si>
+    <t>hotel.viewpage.roomtype.header.taboption</t>
+  </si>
+  <si>
+    <t>booking.confimationpage.headingname</t>
+  </si>
+  <si>
+    <t>Booking Confirmation Details</t>
+  </si>
+  <si>
+    <t>booking.confirmationpage.breakingup.arrow</t>
+  </si>
+  <si>
+    <t>22-November 2017</t>
+  </si>
+  <si>
+    <t>26-November 2017</t>
+  </si>
+  <si>
+    <t>homepage.citylist.optionheader</t>
+  </si>
+  <si>
+    <t>booking.confirmationpage.roomandnights|booking.confirmationpage.servicecharge|booking.confirmationpage.coupon|booking.confirmationpage.promodiscount|booking.confirmationpage.extracost|booking.confirmationpage.totalprice</t>
+  </si>
+  <si>
+    <t>homepage.passenger.room</t>
+  </si>
+  <si>
+    <t>Executed</t>
+  </si>
+  <si>
+    <t>Book Now</t>
+  </si>
+  <si>
+    <t>Please enter an Email Address</t>
+  </si>
+  <si>
+    <t>Username and password doesn't match</t>
+  </si>
+  <si>
+    <t>Jkay@yopmail.com</t>
+  </si>
+  <si>
+    <t>Please enter a password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hey </t>
+  </si>
+  <si>
+    <t>User is not registered</t>
+  </si>
+  <si>
+    <t>verifySuccessMsg1</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>Not Executed</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Please enter a valid Phone Number</t>
+  </si>
+  <si>
+    <t>9985652000</t>
+  </si>
+  <si>
+    <t>9985652007</t>
+  </si>
+  <si>
+    <t>Email already registered !</t>
+  </si>
+  <si>
+    <t>7654qwert</t>
+  </si>
+  <si>
+    <t>Royal Orchid Central</t>
+  </si>
+  <si>
+    <t>booking.confirmationpage.paynowbtn</t>
   </si>
 </sst>
 </file>
@@ -430,7 +541,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -453,6 +564,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -461,7 +583,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -481,6 +603,7 @@
     <xf numFmtId="11" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -802,10 +925,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -813,21 +936,21 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -835,10 +958,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -846,10 +969,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -857,13 +980,13 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -873,10 +996,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F80"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C59" workbookViewId="0">
-      <selection activeCell="H72" sqref="H72"/>
+    <sheetView topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -886,7 +1009,7 @@
     <col min="3" max="3" width="17.42578125" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="42.7109375" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="76.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -911,7 +1034,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
@@ -921,11 +1044,13 @@
         <v>19</v>
       </c>
       <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
+      <c r="F2" s="6" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
@@ -935,11 +1060,13 @@
         <v>20</v>
       </c>
       <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
@@ -949,11 +1076,13 @@
         <v>22</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6" t="s">
@@ -963,71 +1092,83 @@
         <v>22</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="6" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6" t="s">
-        <v>39</v>
+        <v>140</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+        <v>40</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
@@ -1035,11 +1176,13 @@
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
@@ -1049,11 +1192,13 @@
         <v>19</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
@@ -1063,115 +1208,133 @@
         <v>20</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="F14" s="2" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F16" s="2"/>
+        <v>39</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="F18" s="2" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>39</v>
+        <v>140</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+        <v>43</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
@@ -1179,11 +1342,13 @@
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="F20" s="2" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7" t="s">
@@ -1197,7 +1362,7 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="s">
@@ -1211,7 +1376,7 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
@@ -1225,7 +1390,7 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
@@ -1239,7 +1404,7 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
@@ -1253,53 +1418,53 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F27" s="7"/>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
@@ -1311,7 +1476,7 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
@@ -1325,7 +1490,7 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
@@ -1339,111 +1504,111 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E34" s="13" t="s">
         <v>80</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E34" s="13" t="s">
-        <v>81</v>
       </c>
       <c r="F34" s="2"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F35" s="2"/>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F36" s="2"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
@@ -1455,7 +1620,7 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8" t="s">
@@ -1469,7 +1634,7 @@
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8" t="s">
@@ -1483,293 +1648,293 @@
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E43" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F43" s="8"/>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="D45" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="E45" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F45" s="8"/>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D47" s="8"/>
       <c r="E47" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F47" s="8"/>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F49" s="8"/>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F50" s="8"/>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D51" s="8"/>
       <c r="E51" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F51" s="8"/>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E54" s="8"/>
       <c r="F54" s="8"/>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D55" s="8"/>
       <c r="E55" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F55" s="8"/>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E56" s="8"/>
       <c r="F56" s="8"/>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E57" s="8"/>
       <c r="F57" s="8"/>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E58" s="8"/>
       <c r="F58" s="8"/>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B59" s="8"/>
       <c r="C59" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E59" s="8"/>
       <c r="F59" s="8"/>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E60" s="11" t="s">
         <v>75</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="E60" s="11" t="s">
-        <v>76</v>
       </c>
       <c r="F60" s="8"/>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B61" s="8"/>
       <c r="C61" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D61" s="11" t="s">
         <v>78</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>79</v>
       </c>
       <c r="E61" s="11"/>
       <c r="F61" s="8"/>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="8" t="s">
@@ -1781,7 +1946,7 @@
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B63" s="15"/>
       <c r="C63" s="15" t="s">
@@ -1791,11 +1956,13 @@
         <v>19</v>
       </c>
       <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
+      <c r="F63" s="16" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B64" s="15"/>
       <c r="C64" s="15" t="s">
@@ -1805,25 +1972,29 @@
         <v>20</v>
       </c>
       <c r="E64" s="15"/>
-      <c r="F64" s="16"/>
+      <c r="F64" s="16" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B65" s="15"/>
       <c r="C65" s="15" t="s">
         <v>5</v>
       </c>
       <c r="D65" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E65" s="15"/>
-      <c r="F65" s="16"/>
+      <c r="F65" s="16" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B66" s="15"/>
       <c r="C66" s="15" t="s">
@@ -1831,215 +2002,539 @@
       </c>
       <c r="D66" s="15"/>
       <c r="E66" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="F66" s="16"/>
+        <v>86</v>
+      </c>
+      <c r="F66" s="16" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B67" s="15"/>
       <c r="C67" s="15" t="s">
         <v>5</v>
       </c>
       <c r="D67" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E67" s="15"/>
-      <c r="F67" s="16"/>
+      <c r="F67" s="16" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B68" s="15"/>
       <c r="C68" s="15" t="s">
-        <v>49</v>
+        <v>119</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="E68" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="F68" s="16"/>
+        <v>129</v>
+      </c>
+      <c r="E68" s="15"/>
+      <c r="F68" s="16" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B69" s="15"/>
       <c r="C69" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="D69" s="15"/>
-      <c r="E69" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="F69" s="16"/>
+        <v>48</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="E69" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F69" s="16" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B70" s="15"/>
       <c r="C70" s="15" t="s">
-        <v>102</v>
-      </c>
-      <c r="D70" s="15"/>
-      <c r="E70" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="F70" s="16"/>
+        <v>119</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E70" s="15"/>
+      <c r="F70" s="16" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B71" s="15"/>
       <c r="C71" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D71" s="15" t="s">
-        <v>91</v>
-      </c>
-      <c r="E71" s="18"/>
-      <c r="F71" s="16"/>
+        <v>54</v>
+      </c>
+      <c r="D71" s="15"/>
+      <c r="E71" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="F71" s="16" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B72" s="15"/>
       <c r="C72" s="15" t="s">
-        <v>58</v>
+        <v>99</v>
       </c>
       <c r="D72" s="15"/>
-      <c r="E72" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="F72" s="16"/>
+      <c r="E72" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="F72" s="16" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B73" s="15"/>
       <c r="C73" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="D73" s="15"/>
-      <c r="E73" s="18" t="s">
-        <v>92</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="E73" s="17"/>
       <c r="F73" s="16"/>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B74" s="15"/>
       <c r="C74" s="15" t="s">
-        <v>62</v>
+        <v>5</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>57</v>
+        <v>90</v>
       </c>
       <c r="E74" s="18"/>
-      <c r="F74" s="16"/>
+      <c r="F74" s="16" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B75" s="15"/>
       <c r="C75" s="15" t="s">
-        <v>5</v>
+        <v>119</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>66</v>
+        <v>131</v>
       </c>
       <c r="E75" s="18"/>
-      <c r="F75" s="16"/>
+      <c r="F75" s="16" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B76" s="15"/>
       <c r="C76" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="D76" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="E76" s="17" t="s">
-        <v>108</v>
-      </c>
-      <c r="F76" s="16"/>
+        <v>57</v>
+      </c>
+      <c r="D76" s="15"/>
+      <c r="E76" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="F76" s="16" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B77" s="15"/>
       <c r="C77" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="D77" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="E77" s="17"/>
-      <c r="F77" s="16"/>
+        <v>95</v>
+      </c>
+      <c r="D77" s="15"/>
+      <c r="E77" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F77" s="16" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B78" s="15"/>
       <c r="C78" s="15" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="D78" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E78" s="17" t="s">
-        <v>109</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="E78" s="18"/>
       <c r="F78" s="16"/>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B79" s="15"/>
       <c r="C79" s="15" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="D79" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="E79" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="F79" s="16"/>
+        <v>56</v>
+      </c>
+      <c r="E79" s="18"/>
+      <c r="F79" s="16" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B80" s="15"/>
       <c r="C80" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D80" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="E80" s="18"/>
+      <c r="F80" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B81" s="15"/>
+      <c r="C81" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E81" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="F81" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B82" s="15"/>
+      <c r="C82" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="D82" s="15"/>
+      <c r="E82" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="F82" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B83" s="15"/>
+      <c r="C83" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="D83" s="15"/>
+      <c r="E83" s="15"/>
+      <c r="F83" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B84" s="15"/>
+      <c r="C84" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D84" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E84" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="F84" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B85" s="15"/>
+      <c r="C85" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="D85" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="E85" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="F85" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B86" s="15"/>
+      <c r="C86" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D86" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="E86" s="15"/>
+      <c r="F86" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B87" s="15"/>
+      <c r="C87" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D87" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E87" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="F87" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B88" s="15"/>
+      <c r="C88" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D88" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E88" s="15"/>
+      <c r="F88" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B89" s="15"/>
+      <c r="C89" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D89" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="E89" s="15"/>
+      <c r="F89" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B90" s="15"/>
+      <c r="C90" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D90" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="E90" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="F90" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B91" s="15"/>
+      <c r="C91" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D91" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="E91" s="15"/>
+      <c r="F91" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B92" s="15"/>
+      <c r="C92" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D92" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="E92" s="15"/>
+      <c r="F92" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B93" s="15"/>
+      <c r="C93" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="D93" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="E93" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F93" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B94" s="15"/>
+      <c r="C94" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D94" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="E94" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F94" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B95" s="15"/>
+      <c r="C95" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D95" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="D80" s="15" t="s">
+      <c r="E95" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="F95" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B96" s="15"/>
+      <c r="C96" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D96" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="E80" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="F80" s="16"/>
+      <c r="E96" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F96" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B97" s="15"/>
+      <c r="C97" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D97" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="E97" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F97" s="16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B98" s="15"/>
+      <c r="C98" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D98" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="E98" s="15"/>
+      <c r="F98" s="15" t="s">
+        <v>132</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2054,10 +2549,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12:H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2066,7 +2561,7 @@
     <col min="2" max="2" width="29.42578125" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="6.5703125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="17.28515625" hidden="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="16" customWidth="1" collapsed="1"/>
@@ -2074,7 +2569,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2100,16 +2595,28 @@
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
+      <c r="D3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E4" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2117,10 +2624,16 @@
         <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>43</v>
+      <c r="D5" t="s">
+        <v>138</v>
+      </c>
+      <c r="E5" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2129,16 +2642,28 @@
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E6" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5" t="s">
-        <v>26</v>
+        <v>3</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" t="s">
+        <v>137</v>
+      </c>
+      <c r="E7" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2149,12 +2674,18 @@
         <v>11</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2171,7 +2702,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>
@@ -2187,11 +2718,71 @@
       <c r="A12" t="s">
         <v>3</v>
       </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
       <c r="C12" s="5" t="s">
-        <v>95</v>
+        <v>145</v>
+      </c>
+      <c r="D12">
+        <v>12345678</v>
+      </c>
+      <c r="E12" t="s">
+        <v>134</v>
+      </c>
+      <c r="F12" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13">
+        <v>12345678</v>
+      </c>
+      <c r="E13" t="s">
+        <v>144</v>
+      </c>
+      <c r="F13" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E14" t="s">
+        <v>137</v>
+      </c>
+      <c r="F14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D15" t="s">
+        <v>148</v>
+      </c>
+      <c r="E15" t="s">
+        <v>147</v>
+      </c>
+      <c r="F15" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -2200,8 +2791,9 @@
     <hyperlink ref="B5" r:id="rId2"/>
     <hyperlink ref="B4" r:id="rId3"/>
     <hyperlink ref="B8" r:id="rId4"/>
+    <hyperlink ref="B7" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test cases flow changes in keywords file.
</commit_message>
<xml_diff>
--- a/src/main/java/com/hybridframework_Selenium/testdata/Test Suite1.xlsx
+++ b/src/main/java/com/hybridframework_Selenium/testdata/Test Suite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19815" windowHeight="2685" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19815" windowHeight="2685" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="151">
   <si>
     <t>TCID</t>
   </si>
@@ -183,9 +183,6 @@
     <t>chooseDate</t>
   </si>
   <si>
-    <t>20-September 2017</t>
-  </si>
-  <si>
     <t>homepage.passenger</t>
   </si>
   <si>
@@ -255,18 +252,6 @@
     <t>flightreviewpage.basefire|flightreviewpage.feesurcharges|flightreviewpage.grandtotal</t>
   </si>
   <si>
-    <t>directInput</t>
-  </si>
-  <si>
-    <t>jakay577@gmail.com</t>
-  </si>
-  <si>
-    <t>976556767</t>
-  </si>
-  <si>
-    <t>7889</t>
-  </si>
-  <si>
     <t>signUpPageTestcases</t>
   </si>
   <si>
@@ -414,61 +399,76 @@
     <t>homepage.passenger.room</t>
   </si>
   <si>
+    <t>Book Now</t>
+  </si>
+  <si>
+    <t>Please enter an Email Address</t>
+  </si>
+  <si>
+    <t>Username and password doesn't match</t>
+  </si>
+  <si>
+    <t>Jkay@yopmail.com</t>
+  </si>
+  <si>
+    <t>Please enter a password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hey </t>
+  </si>
+  <si>
+    <t>User is not registered</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>Please enter a valid Phone Number</t>
+  </si>
+  <si>
+    <t>9985652000</t>
+  </si>
+  <si>
+    <t>9985652007</t>
+  </si>
+  <si>
+    <t>Email already registered !</t>
+  </si>
+  <si>
+    <t>7654qwert</t>
+  </si>
+  <si>
+    <t>Royal Orchid Central</t>
+  </si>
+  <si>
+    <t>booking.confirmationpage.paynowbtn</t>
+  </si>
+  <si>
+    <t>randomMailgenerator</t>
+  </si>
+  <si>
+    <t>randomPhonenoGenerator</t>
+  </si>
+  <si>
+    <t>priyanka@gmail.com</t>
+  </si>
+  <si>
+    <t>priyanka8911</t>
+  </si>
+  <si>
+    <t>HEY</t>
+  </si>
+  <si>
+    <t>12-October 2017</t>
+  </si>
+  <si>
     <t>Executed</t>
   </si>
   <si>
-    <t>Book Now</t>
-  </si>
-  <si>
-    <t>Please enter an Email Address</t>
-  </si>
-  <si>
-    <t>Username and password doesn't match</t>
-  </si>
-  <si>
-    <t>Jkay@yopmail.com</t>
-  </si>
-  <si>
-    <t>Please enter a password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hey </t>
-  </si>
-  <si>
-    <t>User is not registered</t>
-  </si>
-  <si>
-    <t>verifySuccessMsg1</t>
-  </si>
-  <si>
-    <t>SKIP</t>
-  </si>
-  <si>
     <t>Not Executed</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>Please enter a valid Phone Number</t>
-  </si>
-  <si>
-    <t>9985652000</t>
-  </si>
-  <si>
-    <t>9985652007</t>
-  </si>
-  <si>
-    <t>Email already registered !</t>
-  </si>
-  <si>
-    <t>7654qwert</t>
-  </si>
-  <si>
-    <t>Royal Orchid Central</t>
-  </si>
-  <si>
-    <t>booking.confirmationpage.paynowbtn</t>
   </si>
 </sst>
 </file>
@@ -597,13 +597,13 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -902,7 +902,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -925,65 +925,65 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
         <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B3" t="s">
         <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
         <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
         <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
@@ -998,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F98"/>
   <sheetViews>
-    <sheetView topLeftCell="D13" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="B47" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1034,7 +1034,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
@@ -1044,13 +1044,11 @@
         <v>19</v>
       </c>
       <c r="E2" s="6"/>
-      <c r="F2" s="6" t="s">
-        <v>132</v>
-      </c>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
@@ -1060,13 +1058,11 @@
         <v>20</v>
       </c>
       <c r="E3" s="6"/>
-      <c r="F3" s="6" t="s">
-        <v>132</v>
-      </c>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
@@ -1076,13 +1072,11 @@
         <v>22</v>
       </c>
       <c r="E4" s="6"/>
-      <c r="F4" s="6" t="s">
-        <v>132</v>
-      </c>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6" t="s">
@@ -1092,13 +1086,11 @@
         <v>22</v>
       </c>
       <c r="E5" s="6"/>
-      <c r="F5" s="6" t="s">
-        <v>132</v>
-      </c>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
@@ -1110,13 +1102,11 @@
       <c r="E6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>132</v>
-      </c>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
@@ -1128,13 +1118,11 @@
       <c r="E7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>132</v>
-      </c>
+      <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
@@ -1144,17 +1132,15 @@
         <v>31</v>
       </c>
       <c r="E8" s="6"/>
-      <c r="F8" s="6" t="s">
-        <v>132</v>
-      </c>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6" t="s">
-        <v>140</v>
+        <v>38</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>40</v>
@@ -1162,13 +1148,11 @@
       <c r="E9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>132</v>
-      </c>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" s="6" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B10" s="6"/>
       <c r="C10" s="6" t="s">
@@ -1176,13 +1160,11 @@
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="6" t="s">
-        <v>142</v>
-      </c>
+      <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
@@ -1192,13 +1174,11 @@
         <v>19</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
@@ -1208,13 +1188,11 @@
         <v>20</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
@@ -1224,13 +1202,11 @@
         <v>33</v>
       </c>
       <c r="E13" s="2"/>
-      <c r="F13" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
@@ -1240,13 +1216,11 @@
         <v>33</v>
       </c>
       <c r="E14" s="2"/>
-      <c r="F14" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="F14" s="2"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
@@ -1258,13 +1232,11 @@
       <c r="E15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
@@ -1276,13 +1248,11 @@
       <c r="E16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
@@ -1294,13 +1264,11 @@
       <c r="E17" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="F17" s="2"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
@@ -1310,17 +1278,15 @@
         <v>37</v>
       </c>
       <c r="E18" s="2"/>
-      <c r="F18" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="F18" s="2"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>140</v>
+        <v>38</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>43</v>
@@ -1328,13 +1294,11 @@
       <c r="E19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>132</v>
-      </c>
+      <c r="F19" s="2"/>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
@@ -1342,13 +1306,11 @@
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="2" t="s">
-        <v>142</v>
-      </c>
+      <c r="F20" s="2"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7" t="s">
@@ -1362,7 +1324,7 @@
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="s">
@@ -1376,7 +1338,7 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
@@ -1390,7 +1352,7 @@
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
@@ -1404,7 +1366,7 @@
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
@@ -1418,11 +1380,11 @@
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
-        <v>79</v>
+        <v>6</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>29</v>
@@ -1434,11 +1396,11 @@
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>79</v>
+        <v>6</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>30</v>
@@ -1450,7 +1412,7 @@
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
@@ -1464,7 +1426,7 @@
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7" t="s">
@@ -1476,7 +1438,7 @@
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
@@ -1490,7 +1452,7 @@
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
@@ -1504,7 +1466,7 @@
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
@@ -1518,7 +1480,7 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
@@ -1532,55 +1494,53 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>79</v>
+        <v>143</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E34" s="13" t="s">
-        <v>80</v>
+      <c r="E34" s="19" t="s">
+        <v>145</v>
       </c>
       <c r="F34" s="2"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>79</v>
+        <v>144</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E35" s="14" t="s">
-        <v>81</v>
-      </c>
+      <c r="E35" s="13"/>
       <c r="F35" s="2"/>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
-        <v>79</v>
+        <v>6</v>
       </c>
       <c r="D36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E36" s="14" t="s">
-        <v>82</v>
+      <c r="E36" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="F36" s="2"/>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
@@ -1594,7 +1554,7 @@
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
@@ -1603,12 +1563,14 @@
       <c r="D38" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E38" s="2"/>
+      <c r="E38" s="2" t="s">
+        <v>147</v>
+      </c>
       <c r="F38" s="2"/>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
@@ -1620,7 +1582,7 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8" t="s">
@@ -1630,11 +1592,13 @@
         <v>19</v>
       </c>
       <c r="E40" s="8"/>
-      <c r="F40" s="8"/>
+      <c r="F40" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8" t="s">
@@ -1644,11 +1608,13 @@
         <v>20</v>
       </c>
       <c r="E41" s="8"/>
-      <c r="F41" s="8"/>
+      <c r="F41" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="8" t="s">
@@ -1658,11 +1624,13 @@
         <v>46</v>
       </c>
       <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
+      <c r="F42" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8" t="s">
@@ -1674,11 +1642,13 @@
       <c r="E43" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="F43" s="8"/>
+      <c r="F43" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="8" t="s">
@@ -1688,11 +1658,13 @@
         <v>50</v>
       </c>
       <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
+      <c r="F44" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="8" t="s">
@@ -1704,11 +1676,13 @@
       <c r="E45" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F45" s="8"/>
+      <c r="F45" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="8" t="s">
@@ -1718,11 +1692,13 @@
         <v>53</v>
       </c>
       <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
+      <c r="F46" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="8" t="s">
@@ -1730,211 +1706,237 @@
       </c>
       <c r="D47" s="8"/>
       <c r="E47" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F47" s="8"/>
+        <v>148</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
+      <c r="F48" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F49" s="8"/>
+        <v>65</v>
+      </c>
+      <c r="F49" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F50" s="8"/>
+        <v>66</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D51" s="8"/>
       <c r="E51" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="F51" s="8"/>
+        <v>66</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E52" s="8"/>
-      <c r="F52" s="8"/>
+      <c r="F52" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E53" s="8"/>
-      <c r="F53" s="8"/>
+      <c r="F53" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E54" s="8"/>
-      <c r="F54" s="8"/>
+      <c r="F54" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D55" s="8"/>
       <c r="E55" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F55" s="8"/>
+        <v>63</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="8" t="s">
         <v>5</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E56" s="8"/>
-      <c r="F56" s="8"/>
+      <c r="F56" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E57" s="8"/>
-      <c r="F57" s="8"/>
+      <c r="F57" s="8" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E58" s="8"/>
-      <c r="F58" s="8"/>
+      <c r="F58" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B59" s="8"/>
       <c r="C59" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E59" s="8"/>
-      <c r="F59" s="8"/>
+      <c r="F59" s="8" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="E60" s="11" t="s">
         <v>74</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="E60" s="11" t="s">
-        <v>75</v>
       </c>
       <c r="F60" s="8"/>
     </row>
     <row r="61" spans="1:6">
       <c r="A61" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B61" s="8"/>
       <c r="C61" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="D61" s="11" t="s">
         <v>77</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>78</v>
       </c>
       <c r="E61" s="11"/>
       <c r="F61" s="8"/>
     </row>
     <row r="62" spans="1:6">
       <c r="A62" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B62" s="8"/>
       <c r="C62" s="8" t="s">
@@ -1945,596 +1947,528 @@
       <c r="F62" s="8"/>
     </row>
     <row r="63" spans="1:6">
-      <c r="A63" s="15" t="s">
+      <c r="A63" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B63" s="14"/>
+      <c r="C63" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E63" s="15"/>
+      <c r="F63" s="15"/>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B64" s="14"/>
+      <c r="C64" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E64" s="14"/>
+      <c r="F64" s="15"/>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B65" s="14"/>
+      <c r="C65" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="E65" s="14"/>
+      <c r="F65" s="15"/>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B66" s="14"/>
+      <c r="C66" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="F66" s="15"/>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B67" s="14"/>
+      <c r="C67" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E67" s="14"/>
+      <c r="F67" s="15"/>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B68" s="14"/>
+      <c r="C68" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="E68" s="14"/>
+      <c r="F68" s="15"/>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B69" s="14"/>
+      <c r="C69" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D69" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E69" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F69" s="15"/>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B70" s="14"/>
+      <c r="C70" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D70" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="E70" s="14"/>
+      <c r="F70" s="15"/>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B71" s="14"/>
+      <c r="C71" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D71" s="14"/>
+      <c r="E71" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="F71" s="15"/>
+    </row>
+    <row r="72" spans="1:6">
+      <c r="A72" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B72" s="14"/>
+      <c r="C72" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="B63" s="15"/>
-      <c r="C63" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="D63" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E63" s="16"/>
-      <c r="F63" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6">
-      <c r="A64" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B64" s="15"/>
-      <c r="C64" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="D64" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E64" s="15"/>
-      <c r="F64" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B65" s="15"/>
-      <c r="C65" s="15" t="s">
+      <c r="D72" s="14"/>
+      <c r="E72" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="F72" s="15"/>
+    </row>
+    <row r="73" spans="1:6">
+      <c r="A73" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B73" s="14"/>
+      <c r="C73" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="E73" s="16"/>
+      <c r="F73" s="15"/>
+    </row>
+    <row r="74" spans="1:6">
+      <c r="A74" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B74" s="14"/>
+      <c r="C74" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D65" s="15" t="s">
+      <c r="D74" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="E65" s="15"/>
-      <c r="F65" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B66" s="15"/>
-      <c r="C66" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D66" s="15"/>
-      <c r="E66" s="15" t="s">
+      <c r="E74" s="17"/>
+      <c r="F74" s="15"/>
+    </row>
+    <row r="75" spans="1:6">
+      <c r="A75" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B75" s="14"/>
+      <c r="C75" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="E75" s="17"/>
+      <c r="F75" s="15"/>
+    </row>
+    <row r="76" spans="1:6">
+      <c r="A76" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B76" s="14"/>
+      <c r="C76" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D76" s="14"/>
+      <c r="E76" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F76" s="15"/>
+    </row>
+    <row r="77" spans="1:6">
+      <c r="A77" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B77" s="14"/>
+      <c r="C77" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D77" s="14"/>
+      <c r="E77" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="F66" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B67" s="15"/>
-      <c r="C67" s="15" t="s">
+      <c r="F77" s="15"/>
+    </row>
+    <row r="78" spans="1:6">
+      <c r="A78" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B78" s="14"/>
+      <c r="C78" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D78" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="E78" s="17"/>
+      <c r="F78" s="15"/>
+    </row>
+    <row r="79" spans="1:6">
+      <c r="A79" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B79" s="14"/>
+      <c r="C79" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D79" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E79" s="17"/>
+      <c r="F79" s="15"/>
+    </row>
+    <row r="80" spans="1:6">
+      <c r="A80" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B80" s="14"/>
+      <c r="C80" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D67" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="E67" s="15"/>
-      <c r="F67" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B68" s="15"/>
-      <c r="C68" s="15" t="s">
+      <c r="D80" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E80" s="17"/>
+      <c r="F80" s="15"/>
+    </row>
+    <row r="81" spans="1:6">
+      <c r="A81" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B81" s="14"/>
+      <c r="C81" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D81" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="E81" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="F81" s="15"/>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B82" s="14"/>
+      <c r="C82" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="D82" s="14"/>
+      <c r="E82" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="F82" s="14"/>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B83" s="14"/>
+      <c r="C83" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B84" s="14"/>
+      <c r="C84" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E84" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="F84" s="15"/>
+    </row>
+    <row r="85" spans="1:6">
+      <c r="A85" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B85" s="14"/>
+      <c r="C85" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D85" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E85" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="F85" s="15"/>
+    </row>
+    <row r="86" spans="1:6">
+      <c r="A86" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B86" s="14"/>
+      <c r="C86" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D86" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E86" s="14"/>
+      <c r="F86" s="15"/>
+    </row>
+    <row r="87" spans="1:6">
+      <c r="A87" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B87" s="14"/>
+      <c r="C87" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D87" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E87" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F87" s="15"/>
+    </row>
+    <row r="88" spans="1:6">
+      <c r="A88" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B88" s="14"/>
+      <c r="C88" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D88" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E88" s="14"/>
+      <c r="F88" s="14"/>
+    </row>
+    <row r="89" spans="1:6">
+      <c r="A89" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B89" s="14"/>
+      <c r="C89" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D89" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
+    </row>
+    <row r="90" spans="1:6">
+      <c r="A90" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B90" s="14"/>
+      <c r="C90" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D90" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="D68" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="E68" s="15"/>
-      <c r="F68" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B69" s="15"/>
-      <c r="C69" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="D69" s="15" t="s">
-        <v>88</v>
-      </c>
-      <c r="E69" s="15" t="s">
-        <v>89</v>
-      </c>
-      <c r="F69" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B70" s="15"/>
-      <c r="C70" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="D70" s="15" t="s">
+      <c r="E90" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="F90" s="14"/>
+    </row>
+    <row r="91" spans="1:6">
+      <c r="A91" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B91" s="14"/>
+      <c r="C91" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D91" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="E70" s="15"/>
-      <c r="F70" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B71" s="15"/>
-      <c r="C71" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D71" s="15"/>
-      <c r="E71" s="17" t="s">
-        <v>127</v>
-      </c>
-      <c r="F71" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
-      <c r="A72" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B72" s="15"/>
-      <c r="C72" s="15" t="s">
-        <v>99</v>
-      </c>
-      <c r="D72" s="15"/>
-      <c r="E72" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="F72" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="A73" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B73" s="15"/>
-      <c r="C73" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="D73" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="E73" s="17"/>
-      <c r="F73" s="16"/>
-    </row>
-    <row r="74" spans="1:6">
-      <c r="A74" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B74" s="15"/>
-      <c r="C74" s="15" t="s">
+      <c r="E91" s="14"/>
+      <c r="F91" s="14"/>
+    </row>
+    <row r="92" spans="1:6">
+      <c r="A92" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B92" s="14"/>
+      <c r="C92" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D92" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="E92" s="14"/>
+      <c r="F92" s="14"/>
+    </row>
+    <row r="93" spans="1:6">
+      <c r="A93" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B93" s="14"/>
+      <c r="C93" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D93" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="E93" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="F93" s="14"/>
+    </row>
+    <row r="94" spans="1:6">
+      <c r="A94" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B94" s="14"/>
+      <c r="C94" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D94" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="E94" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="F94" s="14"/>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B95" s="14"/>
+      <c r="C95" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D95" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E95" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="F95" s="14"/>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B96" s="14"/>
+      <c r="C96" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E96" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="F96" s="14"/>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B97" s="14"/>
+      <c r="C97" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E97" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="F97" s="15"/>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B98" s="14"/>
+      <c r="C98" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D74" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="E74" s="18"/>
-      <c r="F74" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
-      <c r="A75" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B75" s="15"/>
-      <c r="C75" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="D75" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="E75" s="18"/>
-      <c r="F75" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B76" s="15"/>
-      <c r="C76" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D76" s="15"/>
-      <c r="E76" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="F76" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B77" s="15"/>
-      <c r="C77" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="D77" s="15"/>
-      <c r="E77" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="F77" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B78" s="15"/>
-      <c r="C78" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="D78" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="E78" s="18"/>
-      <c r="F78" s="16"/>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B79" s="15"/>
-      <c r="C79" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="D79" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="E79" s="18"/>
-      <c r="F79" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
-      <c r="A80" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B80" s="15"/>
-      <c r="C80" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D80" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="E80" s="18"/>
-      <c r="F80" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6">
-      <c r="A81" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B81" s="15"/>
-      <c r="C81" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="D81" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="E81" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="F81" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6">
-      <c r="A82" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B82" s="15"/>
-      <c r="C82" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="D82" s="15"/>
-      <c r="E82" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="F82" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6">
-      <c r="A83" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B83" s="15"/>
-      <c r="C83" s="15" t="s">
-        <v>106</v>
-      </c>
-      <c r="D83" s="15"/>
-      <c r="E83" s="15"/>
-      <c r="F83" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6">
-      <c r="A84" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B84" s="15"/>
-      <c r="C84" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="D84" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E84" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="F84" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6">
-      <c r="A85" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B85" s="15"/>
-      <c r="C85" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="D85" s="15" t="s">
-        <v>104</v>
-      </c>
-      <c r="E85" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="F85" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6">
-      <c r="A86" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B86" s="15"/>
-      <c r="C86" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D86" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="E86" s="15"/>
-      <c r="F86" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6">
-      <c r="A87" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B87" s="15"/>
-      <c r="C87" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="D87" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="E87" s="15" t="s">
-        <v>133</v>
-      </c>
-      <c r="F87" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6">
-      <c r="A88" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B88" s="15"/>
-      <c r="C88" s="15" t="s">
-        <v>118</v>
-      </c>
-      <c r="D88" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="E88" s="15"/>
-      <c r="F88" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6">
-      <c r="A89" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B89" s="15"/>
-      <c r="C89" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D89" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="E89" s="15"/>
-      <c r="F89" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6">
-      <c r="A90" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B90" s="15"/>
-      <c r="C90" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="D90" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="E90" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="F90" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6">
-      <c r="A91" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B91" s="15"/>
-      <c r="C91" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D91" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="E91" s="15"/>
-      <c r="F91" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6">
-      <c r="A92" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B92" s="15"/>
-      <c r="C92" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="D92" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="E92" s="15"/>
-      <c r="F92" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6">
-      <c r="A93" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B93" s="15"/>
-      <c r="C93" s="15" t="s">
-        <v>109</v>
-      </c>
-      <c r="D93" s="15" t="s">
-        <v>110</v>
-      </c>
-      <c r="E93" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="F93" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6">
-      <c r="A94" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B94" s="15"/>
-      <c r="C94" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D94" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="E94" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="F94" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6">
-      <c r="A95" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B95" s="15"/>
-      <c r="C95" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D95" s="15" t="s">
-        <v>112</v>
-      </c>
-      <c r="E95" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="F95" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
-      <c r="A96" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B96" s="15"/>
-      <c r="C96" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D96" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="E96" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="F96" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
-      <c r="A97" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B97" s="15"/>
-      <c r="C97" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="D97" s="15" t="s">
-        <v>114</v>
-      </c>
-      <c r="E97" s="15" t="s">
-        <v>115</v>
-      </c>
-      <c r="F97" s="16" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
-      <c r="A98" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="B98" s="15"/>
-      <c r="C98" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D98" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="E98" s="15"/>
-      <c r="F98" s="15" t="s">
-        <v>132</v>
-      </c>
+      <c r="D98" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="E98" s="14"/>
+      <c r="F98" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2551,8 +2485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2569,7 +2503,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2596,10 +2530,10 @@
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" t="s">
         <v>134</v>
-      </c>
-      <c r="E3" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2613,10 +2547,10 @@
         <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E4" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2630,10 +2564,10 @@
         <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E5" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2645,10 +2579,10 @@
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E6" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2656,14 +2590,14 @@
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E7" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2677,15 +2611,15 @@
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E8" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2719,16 +2653,16 @@
         <v>3</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="D12">
         <v>12345678</v>
       </c>
       <c r="E12" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F12" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2742,10 +2676,10 @@
         <v>12345678</v>
       </c>
       <c r="E13" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="F13" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2756,13 +2690,13 @@
         <v>41</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E14" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="F14" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2773,16 +2707,16 @@
         <v>41</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D15" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="E15" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="F15" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the new test case and changed old test cases
</commit_message>
<xml_diff>
--- a/src/main/java/com/hybridframework_Selenium/testdata/Test Suite1.xlsx
+++ b/src/main/java/com/hybridframework_Selenium/testdata/Test Suite1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19815" windowHeight="2685" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="19815" windowHeight="2685" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="159">
   <si>
     <t>TCID</t>
   </si>
@@ -84,9 +84,6 @@
     <t>login_link</t>
   </si>
   <si>
-    <t>close</t>
-  </si>
-  <si>
     <t>hjkhjhdjd^7</t>
   </si>
   <si>
@@ -264,9 +261,6 @@
     <t>homepage.hotel.city.hoteloptions</t>
   </si>
   <si>
-    <t>Bangalore</t>
-  </si>
-  <si>
     <t>homepage.hotel.roomguests</t>
   </si>
   <si>
@@ -303,24 +297,15 @@
     <t>listingpage.hotelpageheading</t>
   </si>
   <si>
-    <t>Hotels in Bangalore</t>
-  </si>
-  <si>
     <t>verifyTextPresent</t>
   </si>
   <si>
     <t>hotel.viewpage.hotelname</t>
   </si>
   <si>
-    <t>clickOngivenName</t>
-  </si>
-  <si>
     <t>switchtoWindow</t>
   </si>
   <si>
-    <t>hotel.viewpage.roomonly.bookbtn</t>
-  </si>
-  <si>
     <t>verify_BookingConfirmationDetailsprice</t>
   </si>
   <si>
@@ -369,21 +354,9 @@
     <t>hotel.viewpage.roomtype.header.taboption</t>
   </si>
   <si>
-    <t>booking.confimationpage.headingname</t>
-  </si>
-  <si>
-    <t>Booking Confirmation Details</t>
-  </si>
-  <si>
     <t>booking.confirmationpage.breakingup.arrow</t>
   </si>
   <si>
-    <t>22-November 2017</t>
-  </si>
-  <si>
-    <t>26-November 2017</t>
-  </si>
-  <si>
     <t>homepage.citylist.optionheader</t>
   </si>
   <si>
@@ -393,9 +366,6 @@
     <t>homepage.passenger.room</t>
   </si>
   <si>
-    <t>Book Now</t>
-  </si>
-  <si>
     <t>Please enter an Email Address</t>
   </si>
   <si>
@@ -435,9 +405,6 @@
     <t>7654qwert</t>
   </si>
   <si>
-    <t>Royal Orchid Central</t>
-  </si>
-  <si>
     <t>booking.confirmationpage.paynowbtn</t>
   </si>
   <si>
@@ -465,10 +432,67 @@
     <t>MakeMyTrip - #1 Travel Website 50% OFF on Hotels, Flights &amp; Holiday</t>
   </si>
   <si>
+    <t>closeAnyadverdisement</t>
+  </si>
+  <si>
+    <t>homepage.screenadd.framename|homepage.screenadd.close</t>
+  </si>
+  <si>
+    <t>afterloginusername</t>
+  </si>
+  <si>
     <t>Executed</t>
   </si>
   <si>
     <t>Not Executed</t>
+  </si>
+  <si>
+    <t>12-November 2017</t>
+  </si>
+  <si>
+    <t>20-November 2017</t>
+  </si>
+  <si>
+    <t>Hotels in Mumbai</t>
+  </si>
+  <si>
+    <t>The Park Navi Mumbai</t>
+  </si>
+  <si>
+    <t>hotelRandomSelectTestCase</t>
+  </si>
+  <si>
+    <t>randomSelectWithFilter</t>
+  </si>
+  <si>
+    <t>waitForVisibilityOfElement</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>clickOnFirstHotel</t>
+  </si>
+  <si>
+    <t>listingpage.hotelnamelist</t>
+  </si>
+  <si>
+    <t>2|1|1</t>
+  </si>
+  <si>
+    <t>booking.confirmationpage.totaltxt</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>testing for hotel search listing page select the hotal randomly</t>
+  </si>
+  <si>
+    <t>hotel.viewpage.roomonly.bookbtn|hotel.viewpage.roomonly.bookbtn1</t>
+  </si>
+  <si>
+    <t>clickWhichElementPresent</t>
   </si>
 </sst>
 </file>
@@ -492,7 +516,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -541,6 +565,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -584,7 +614,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -605,6 +635,14 @@
     <xf numFmtId="49" fontId="0" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -900,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -926,10 +964,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -937,10 +975,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -948,10 +986,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -959,21 +997,21 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
         <v>3</v>
@@ -981,13 +1019,24 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C7" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -997,10 +1046,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F98"/>
+  <dimension ref="A1:F115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:A39"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1035,7 +1084,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
@@ -1046,12 +1095,12 @@
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6" t="s">
@@ -1062,12 +1111,12 @@
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" s="6"/>
       <c r="C4" s="6" t="s">
@@ -1078,12 +1127,12 @@
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6" t="s">
@@ -1094,698 +1143,730 @@
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B9" s="6"/>
       <c r="C9" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6" t="s">
-        <v>150</v>
+      <c r="A10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="2"/>
+        <v>17</v>
+      </c>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>137</v>
+      </c>
       <c r="F12" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="F13" s="2"/>
+        <v>18</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="F15" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>9</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F19" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>149</v>
+      <c r="A20" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2" t="s">
-        <v>150</v>
+      <c r="A21" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>39</v>
+      </c>
       <c r="F24" s="7" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="7"/>
+        <v>28</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="F25" s="7" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>40</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="E26" s="7"/>
       <c r="F26" s="7" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7" t="s">
-        <v>6</v>
+        <v>91</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>41</v>
+        <v>140</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>134</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7" t="s">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E28" s="7"/>
+        <v>140</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>134</v>
+      </c>
       <c r="F28" s="7" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7" t="s">
-        <v>150</v>
+      <c r="A29" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="F30" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2" t="s">
-        <v>16</v>
+        <v>138</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>20</v>
+        <v>139</v>
       </c>
       <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+      <c r="F31" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
+      <c r="F32" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
+      <c r="F33" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E34" s="19" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="F34" s="2"/>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E35" s="13"/>
-      <c r="F35" s="2"/>
+      <c r="F35" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E36" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="F36" s="2"/>
+        <v>133</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
+      <c r="F37" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F38" s="2"/>
+        <v>134</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B39" s="2"/>
-      <c r="C39" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D39" s="2"/>
-      <c r="E39" s="2"/>
-      <c r="F39" s="2"/>
+      <c r="A39" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E39" s="8"/>
+      <c r="F39" s="8" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E40" s="8"/>
       <c r="F40" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="E41" s="8"/>
       <c r="F41" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B42" s="8"/>
       <c r="C42" s="8" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="D42" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="E42" s="8"/>
+      <c r="E42" s="8" t="s">
+        <v>49</v>
+      </c>
       <c r="F42" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B43" s="8"/>
       <c r="C43" s="8" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>50</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="E43" s="8"/>
       <c r="F43" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B44" s="8"/>
       <c r="C44" s="8" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E44" s="8"/>
+        <v>47</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="F44" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:6">
       <c r="A45" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="8" t="s">
-        <v>47</v>
+        <v>5</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="E45" s="8" t="s">
         <v>51</v>
       </c>
+      <c r="E45" s="8"/>
       <c r="F45" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B46" s="8"/>
       <c r="C46" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D46" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E46" s="8"/>
+      <c r="D46" s="8"/>
+      <c r="E46" s="9" t="s">
+        <v>135</v>
+      </c>
       <c r="F46" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B47" s="8"/>
       <c r="C47" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D47" s="8"/>
-      <c r="E47" s="9" t="s">
-        <v>146</v>
-      </c>
+      <c r="E47" s="8"/>
       <c r="F47" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B48" s="8"/>
       <c r="C48" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D48" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E48" s="8"/>
+      <c r="D48" s="8"/>
+      <c r="E48" s="10" t="s">
+        <v>63</v>
+      </c>
       <c r="F48" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:6">
       <c r="A49" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B49" s="8"/>
       <c r="C49" s="8" t="s">
@@ -1796,12 +1877,12 @@
         <v>64</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="1:6">
       <c r="A50" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8" t="s">
@@ -1809,799 +1890,1031 @@
       </c>
       <c r="D50" s="8"/>
       <c r="E50" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="D51" s="8"/>
-      <c r="E51" s="10" t="s">
-        <v>65</v>
-      </c>
+      <c r="E51" s="8"/>
       <c r="F51" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E52" s="8"/>
       <c r="F52" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D53" s="8" t="s">
         <v>59</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>54</v>
       </c>
       <c r="E53" s="8"/>
       <c r="F53" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D54" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E54" s="8"/>
+      <c r="D54" s="8"/>
+      <c r="E54" s="8" t="s">
+        <v>61</v>
+      </c>
       <c r="F54" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:6">
       <c r="A55" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="D55" s="8"/>
-      <c r="E55" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="8" t="s">
         <v>62</v>
       </c>
+      <c r="E55" s="8"/>
       <c r="F55" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:6">
       <c r="A56" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B56" s="8"/>
       <c r="C56" s="8" t="s">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E56" s="8"/>
       <c r="F56" s="8" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B57" s="8"/>
       <c r="C57" s="8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E57" s="8"/>
       <c r="F57" s="8" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B58" s="8"/>
       <c r="C58" s="8" t="s">
         <v>70</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E58" s="8"/>
       <c r="F58" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B59" s="8"/>
       <c r="C59" s="8" t="s">
         <v>71</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="E59" s="8"/>
+        <v>73</v>
+      </c>
+      <c r="E59" s="11" t="s">
+        <v>72</v>
+      </c>
       <c r="F59" s="8" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B60" s="8"/>
       <c r="C60" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D60" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="E60" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F60" s="8" t="s">
-        <v>149</v>
-      </c>
+      <c r="D60" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="E60" s="11"/>
+      <c r="F60" s="8"/>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B61" s="8"/>
-      <c r="C61" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="E61" s="11"/>
-      <c r="F61" s="8"/>
+      <c r="A61" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" s="14"/>
+      <c r="C61" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E61" s="15"/>
+      <c r="F61" s="15" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D62" s="11"/>
-      <c r="E62" s="11"/>
-      <c r="F62" s="8" t="s">
-        <v>150</v>
+      <c r="A62" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="B62" s="14"/>
+      <c r="C62" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E62" s="14"/>
+      <c r="F62" s="15" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B63" s="14"/>
       <c r="C63" s="14" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D63" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="E63" s="15"/>
+        <v>77</v>
+      </c>
+      <c r="E63" s="14"/>
       <c r="F63" s="15" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B64" s="14"/>
       <c r="C64" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="D64" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E64" s="14"/>
+        <v>17</v>
+      </c>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14" t="s">
+        <v>78</v>
+      </c>
       <c r="F64" s="15" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" spans="1:6">
       <c r="A65" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B65" s="14"/>
       <c r="C65" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D65" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E65" s="14"/>
       <c r="F65" s="15" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B66" s="14"/>
       <c r="C66" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14" t="s">
-        <v>79</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="D66" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="E66" s="14"/>
       <c r="F66" s="15" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B67" s="14"/>
       <c r="C67" s="14" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="D67" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="E67" s="14"/>
+      <c r="E67" s="14" t="s">
+        <v>50</v>
+      </c>
       <c r="F67" s="15" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B68" s="14"/>
       <c r="C68" s="14" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D68" s="14" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
       <c r="E68" s="14"/>
       <c r="F68" s="15" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B69" s="14"/>
       <c r="C69" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D69" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="E69" s="14" t="s">
-        <v>82</v>
+        <v>52</v>
+      </c>
+      <c r="D69" s="14"/>
+      <c r="E69" s="16" t="s">
+        <v>143</v>
       </c>
       <c r="F69" s="15" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B70" s="14"/>
       <c r="C70" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="D70" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="E70" s="14"/>
+        <v>90</v>
+      </c>
+      <c r="D70" s="14"/>
+      <c r="E70" s="16" t="s">
+        <v>144</v>
+      </c>
       <c r="F70" s="15" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B71" s="14"/>
       <c r="C71" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D71" s="14"/>
-      <c r="E71" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="F71" s="15" t="s">
-        <v>149</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="D71" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="E71" s="16"/>
+      <c r="F71" s="15"/>
     </row>
     <row r="72" spans="1:6">
       <c r="A72" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B72" s="14"/>
       <c r="C72" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="D72" s="14"/>
-      <c r="E72" s="16" t="s">
-        <v>121</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="E72" s="17"/>
       <c r="F72" s="15" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B73" s="14"/>
       <c r="C73" s="14" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D73" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="E73" s="16"/>
-      <c r="F73" s="15"/>
+        <v>115</v>
+      </c>
+      <c r="E73" s="17"/>
+      <c r="F73" s="15" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="74" spans="1:6">
       <c r="A74" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B74" s="14"/>
       <c r="C74" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D74" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="E74" s="17"/>
+        <v>54</v>
+      </c>
+      <c r="D74" s="14"/>
+      <c r="E74" s="17" t="s">
+        <v>63</v>
+      </c>
       <c r="F74" s="15" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:6">
       <c r="A75" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B75" s="14"/>
       <c r="C75" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="D75" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="E75" s="17"/>
+        <v>86</v>
+      </c>
+      <c r="D75" s="14"/>
+      <c r="E75" s="17" t="s">
+        <v>153</v>
+      </c>
       <c r="F75" s="15" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B76" s="14"/>
       <c r="C76" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D76" s="14"/>
-      <c r="E76" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="F76" s="15" t="s">
-        <v>149</v>
-      </c>
+        <v>108</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="E76" s="17"/>
+      <c r="F76" s="15"/>
     </row>
     <row r="77" spans="1:6">
       <c r="A77" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B77" s="14"/>
       <c r="C77" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="D77" s="14"/>
-      <c r="E77" s="17" t="s">
-        <v>84</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="D77" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="E77" s="17"/>
       <c r="F77" s="15" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B78" s="14"/>
       <c r="C78" s="14" t="s">
-        <v>113</v>
+        <v>5</v>
       </c>
       <c r="D78" s="14" t="s">
-        <v>115</v>
+        <v>62</v>
       </c>
       <c r="E78" s="17"/>
-      <c r="F78" s="15"/>
+      <c r="F78" s="15" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B79" s="14"/>
       <c r="C79" s="14" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E79" s="17"/>
+        <v>92</v>
+      </c>
+      <c r="E79" s="16" t="s">
+        <v>145</v>
+      </c>
       <c r="F79" s="15" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B80" s="14"/>
       <c r="C80" s="14" t="s">
-        <v>5</v>
+        <v>151</v>
       </c>
       <c r="D80" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E80" s="17"/>
-      <c r="F80" s="15" t="s">
-        <v>149</v>
+        <v>152</v>
+      </c>
+      <c r="E80" s="14"/>
+      <c r="F80" s="14" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B81" s="14"/>
       <c r="C81" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="D81" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="E81" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="F81" s="15" t="s">
-        <v>149</v>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B82" s="14"/>
       <c r="C82" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D82" s="14"/>
-      <c r="E82" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="F82" s="14" t="s">
         <v>149</v>
+      </c>
+      <c r="D82" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E82" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="F82" s="15" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B83" s="14"/>
       <c r="C83" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="D83" s="14"/>
+        <v>5</v>
+      </c>
+      <c r="D83" s="14" t="s">
+        <v>111</v>
+      </c>
       <c r="E83" s="14"/>
-      <c r="F83" s="14" t="s">
-        <v>149</v>
+      <c r="F83" s="15" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="84" spans="1:6">
       <c r="A84" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B84" s="14"/>
       <c r="C84" s="14" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="D84" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="E84" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="F84" s="15" t="s">
-        <v>149</v>
+        <v>157</v>
+      </c>
+      <c r="E84" s="14"/>
+      <c r="F84" s="14" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B85" s="14"/>
       <c r="C85" s="14" t="s">
-        <v>96</v>
+        <v>158</v>
       </c>
       <c r="D85" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="E85" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="F85" s="15" t="s">
-        <v>149</v>
+        <v>157</v>
+      </c>
+      <c r="E85" s="14"/>
+      <c r="F85" s="14" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B86" s="14"/>
       <c r="C86" s="14" t="s">
-        <v>5</v>
+        <v>91</v>
       </c>
       <c r="D86" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="E86" s="14"/>
-      <c r="F86" s="15" t="s">
-        <v>149</v>
+        <v>154</v>
+      </c>
+      <c r="E86" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="F86" s="14" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B87" s="14"/>
       <c r="C87" s="14" t="s">
-        <v>93</v>
+        <v>5</v>
       </c>
       <c r="D87" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="E87" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="F87" s="15" t="s">
-        <v>149</v>
+        <v>112</v>
+      </c>
+      <c r="E87" s="14"/>
+      <c r="F87" s="14" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B88" s="14"/>
       <c r="C88" s="14" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="D88" s="14" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="E88" s="14"/>
       <c r="F88" s="14" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B89" s="14"/>
       <c r="C89" s="14" t="s">
-        <v>5</v>
+        <v>97</v>
       </c>
       <c r="D89" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="E89" s="14"/>
+        <v>98</v>
+      </c>
+      <c r="E89" s="14" t="s">
+        <v>105</v>
+      </c>
       <c r="F89" s="14" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B90" s="14"/>
       <c r="C90" s="14" t="s">
-        <v>93</v>
+        <v>6</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="E90" s="14" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="F90" s="14" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B91" s="14"/>
       <c r="C91" s="14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D91" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="E91" s="14"/>
+        <v>100</v>
+      </c>
+      <c r="E91" s="14" t="s">
+        <v>104</v>
+      </c>
       <c r="F91" s="14" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B92" s="14"/>
       <c r="C92" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D92" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="D92" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="E92" s="14"/>
+      <c r="E92" s="14" t="s">
+        <v>103</v>
+      </c>
       <c r="F92" s="14" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B93" s="14"/>
       <c r="C93" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D93" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="D93" s="14" t="s">
+      <c r="E93" s="14" t="s">
         <v>103</v>
       </c>
-      <c r="E93" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="F93" s="14" t="s">
-        <v>149</v>
+      <c r="F93" s="15" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B94" s="14"/>
       <c r="C94" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D94" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="E94" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D94" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="E94" s="14"/>
+      <c r="F94" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6">
+      <c r="A95" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B95" s="20"/>
+      <c r="C95" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D95" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E95" s="21"/>
+      <c r="F95" s="21"/>
+    </row>
+    <row r="96" spans="1:6">
+      <c r="A96" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B96" s="20"/>
+      <c r="C96" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D96" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E96" s="20"/>
+      <c r="F96" s="21"/>
+    </row>
+    <row r="97" spans="1:6">
+      <c r="A97" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B97" s="20"/>
+      <c r="C97" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D97" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E97" s="20"/>
+      <c r="F97" s="21"/>
+    </row>
+    <row r="98" spans="1:6">
+      <c r="A98" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B98" s="20"/>
+      <c r="C98" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D98" s="20"/>
+      <c r="E98" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="F98" s="21"/>
+    </row>
+    <row r="99" spans="1:6">
+      <c r="A99" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B99" s="20"/>
+      <c r="C99" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D99" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="E99" s="20"/>
+      <c r="F99" s="21"/>
+    </row>
+    <row r="100" spans="1:6">
+      <c r="A100" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B100" s="20"/>
+      <c r="C100" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D100" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="E100" s="20"/>
+      <c r="F100" s="21"/>
+    </row>
+    <row r="101" spans="1:6">
+      <c r="A101" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B101" s="20"/>
+      <c r="C101" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="D101" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="E101" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="F101" s="21"/>
+    </row>
+    <row r="102" spans="1:6">
+      <c r="A102" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B102" s="20"/>
+      <c r="C102" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D102" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="F94" s="14" t="s">
+      <c r="E102" s="20"/>
+      <c r="F102" s="21"/>
+    </row>
+    <row r="103" spans="1:6">
+      <c r="A103" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B103" s="20"/>
+      <c r="C103" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D103" s="20"/>
+      <c r="E103" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="F103" s="21"/>
+    </row>
+    <row r="104" spans="1:6">
+      <c r="A104" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B104" s="20"/>
+      <c r="C104" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="D104" s="20"/>
+      <c r="E104" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="F104" s="21"/>
+    </row>
+    <row r="105" spans="1:6">
+      <c r="A105" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B105" s="20"/>
+      <c r="C105" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D105" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="E105" s="22"/>
+      <c r="F105" s="21"/>
+    </row>
+    <row r="106" spans="1:6">
+      <c r="A106" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B106" s="20"/>
+      <c r="C106" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D106" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="E106" s="23"/>
+      <c r="F106" s="21"/>
+    </row>
+    <row r="107" spans="1:6">
+      <c r="A107" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B107" s="20"/>
+      <c r="C107" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="D107" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="E107" s="23"/>
+      <c r="F107" s="21"/>
+    </row>
+    <row r="108" spans="1:6">
+      <c r="A108" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B108" s="20"/>
+      <c r="C108" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D108" s="20"/>
+      <c r="E108" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="F108" s="21"/>
+    </row>
+    <row r="109" spans="1:6">
+      <c r="A109" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B109" s="20"/>
+      <c r="C109" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="D109" s="20"/>
+      <c r="E109" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F109" s="21"/>
+    </row>
+    <row r="110" spans="1:6">
+      <c r="A110" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B110" s="20"/>
+      <c r="C110" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="D110" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="E110" s="23"/>
+      <c r="F110" s="21"/>
+    </row>
+    <row r="111" spans="1:6">
+      <c r="A111" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B111" s="20"/>
+      <c r="C111" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D111" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E111" s="23"/>
+      <c r="F111" s="21"/>
+    </row>
+    <row r="112" spans="1:6">
+      <c r="A112" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B112" s="20"/>
+      <c r="C112" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D112" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E112" s="23"/>
+      <c r="F112" s="21"/>
+    </row>
+    <row r="113" spans="1:6">
+      <c r="A113" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B113" s="20"/>
+      <c r="C113" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="D113" s="20"/>
+      <c r="E113" s="23"/>
+      <c r="F113" s="21"/>
+    </row>
+    <row r="114" spans="1:6">
+      <c r="A114" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B114" s="20"/>
+      <c r="C114" s="24" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="95" spans="1:6">
-      <c r="A95" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B95" s="14"/>
-      <c r="C95" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D95" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="E95" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="F95" s="14" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6">
-      <c r="A96" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B96" s="14"/>
-      <c r="C96" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D96" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="E96" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="F96" s="14" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6">
-      <c r="A97" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B97" s="14"/>
-      <c r="C97" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D97" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="E97" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="F97" s="15" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6">
-      <c r="A98" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="B98" s="14"/>
-      <c r="C98" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D98" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="E98" s="14"/>
-      <c r="F98" s="14" t="s">
-        <v>149</v>
-      </c>
+      <c r="D114" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="E114" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="F114" s="26"/>
+    </row>
+    <row r="115" spans="1:6">
+      <c r="A115" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="B115" s="14"/>
+      <c r="C115" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="D115" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="E115" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="F115" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E26" r:id="rId50"/>
-    <hyperlink ref="E27" r:id="rId51"/>
-    <hyperlink ref="E34" r:id="rId52"/>
+    <hyperlink ref="E24" r:id="rId455"/>
+    <hyperlink ref="E25" r:id="rId456"/>
+    <hyperlink ref="E34" r:id="rId457"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -2612,8 +2925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2630,7 +2943,7 @@
   <sheetData>
     <row r="1" spans="1:7" s="3" customFormat="1">
       <c r="A1" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -2657,10 +2970,10 @@
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="E3" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -2668,16 +2981,16 @@
         <v>12</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="E4" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2685,16 +2998,16 @@
         <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="D5" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E5" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -2703,13 +3016,13 @@
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="E6" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -2717,14 +3030,14 @@
         <v>3</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="E7" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -2735,18 +3048,18 @@
         <v>11</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="E8" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -2763,7 +3076,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>9</v>
@@ -2780,16 +3093,16 @@
         <v>3</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D12">
         <v>12345678</v>
       </c>
       <c r="E12" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="F12" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -2797,16 +3110,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D13">
         <v>12345678</v>
       </c>
       <c r="E13" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="F13" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -2814,16 +3127,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="E14" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="F14" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2831,28 +3144,28 @@
         <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D15" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="E15" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="F15" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId82"/>
-    <hyperlink ref="B5" r:id="rId83"/>
-    <hyperlink ref="B4" r:id="rId84"/>
-    <hyperlink ref="B8" r:id="rId85"/>
-    <hyperlink ref="B7" r:id="rId86"/>
+    <hyperlink ref="C5" r:id="rId757"/>
+    <hyperlink ref="B5" r:id="rId758"/>
+    <hyperlink ref="B4" r:id="rId759"/>
+    <hyperlink ref="B8" r:id="rId760"/>
+    <hyperlink ref="B7" r:id="rId761"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId6"/>

</xml_diff>